<commit_message>
update results for SOL vs BEL
</commit_message>
<xml_diff>
--- a/output/Results table.xlsx
+++ b/output/Results table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>species</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>BEL BT</t>
   </si>
 </sst>
 </file>
@@ -207,24 +210,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.6581632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="28.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,6 +322,44 @@
         <v>20</v>
       </c>
       <c r="L3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1.729352</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>-0.006369</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.455329</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.265</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>-92.00044</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>21</v>
       </c>
     </row>
@@ -349,7 +390,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -375,7 +416,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>